<commit_message>
min and max problem
</commit_message>
<xml_diff>
--- a/Docs/Vaccines Dashboard Phase 1 Data v2/Stock Management/2018_Vax_Supplied-values.xlsx
+++ b/Docs/Vaccines Dashboard Phase 1 Data v2/Stock Management/2018_Vax_Supplied-values.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BWamala\Desktop\B&amp;R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\vc\Docs\Vaccines Dashboard Phase 1 Data v2\Stock Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="380" yWindow="130" windowWidth="17220" windowHeight="3130" activeTab="7"/>
+    <workbookView xWindow="380" yWindow="130" windowWidth="17220" windowHeight="3130"/>
   </bookViews>
   <sheets>
     <sheet name="IPV" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="134">
   <si>
     <t>Wastage factor</t>
   </si>
@@ -426,6 +426,9 @@
   <si>
     <t>Min</t>
   </si>
+  <si>
+    <t>2018 Min and Max</t>
+  </si>
 </sst>
 </file>
 
@@ -784,14 +787,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:G118"/>
+  <dimension ref="A2:G118"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B118"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+    </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>121</v>
@@ -5686,7 +5694,7 @@
   <dimension ref="A4:G118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:G118"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12185,8 +12193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:G118"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>